<commit_message>
TP3 - Complejidad Computacional
Se actualiza la funcion recursiva par, los tests y las estadisticas
finales.
</commit_message>
<xml_diff>
--- a/TPs/3 - Complejidad Computacional/Estadisticas.xlsx
+++ b/TPs/3 - Complejidad Computacional/Estadisticas.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignal\Desktop\Ignacio\UNLaM\Programación Avanzada\TP\workspace\TP3 - 2DA ENTREGA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauro\Documents\GitHub\ProgramacionAvanzada\TPs\3 - Complejidad Computacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Polinomio 5" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,13 @@
     <t>O(n)</t>
   </si>
   <si>
-    <t>Conclusión: los métodos más eficaces son los que utilizan programación dinámica.</t>
-  </si>
-  <si>
     <t>O(1)</t>
   </si>
   <si>
     <t>O(n ln n)</t>
+  </si>
+  <si>
+    <t>Conclusión: los métodos más eficaces son los que utilizan programación dinámica y la recursiva par.</t>
   </si>
 </sst>
 </file>
@@ -292,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -323,6 +323,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -712,37 +713,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>28</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>52</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>130</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>146</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>218</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>294</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>340</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1428,7 +1429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1463,7 +1464,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1650,21 +1651,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1809,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -1835,7 +1836,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9" s="5">
         <v>0</v>
@@ -1861,7 +1862,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F10" s="5">
         <v>0</v>
@@ -1887,7 +1888,7 @@
         <v>28</v>
       </c>
       <c r="E11" s="5">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="F11" s="5">
         <v>0</v>
@@ -1913,7 +1914,7 @@
         <v>54</v>
       </c>
       <c r="E12" s="5">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -1938,8 +1939,8 @@
       <c r="D13" s="5">
         <v>90</v>
       </c>
-      <c r="E13" s="5">
-        <v>82</v>
+      <c r="E13" s="16">
+        <v>2</v>
       </c>
       <c r="F13" s="5">
         <v>0</v>
@@ -1965,7 +1966,7 @@
         <v>138</v>
       </c>
       <c r="E14" s="5">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="F14" s="5">
         <v>0</v>
@@ -1991,7 +1992,7 @@
         <v>156</v>
       </c>
       <c r="E15" s="5">
-        <v>146</v>
+        <v>2</v>
       </c>
       <c r="F15" s="5">
         <v>0</v>
@@ -2017,7 +2018,7 @@
         <v>225</v>
       </c>
       <c r="E16" s="5">
-        <v>218</v>
+        <v>3</v>
       </c>
       <c r="F16" s="5">
         <v>0</v>
@@ -2043,7 +2044,7 @@
         <v>268</v>
       </c>
       <c r="E17" s="5">
-        <v>294</v>
+        <v>3</v>
       </c>
       <c r="F17" s="5">
         <v>0</v>
@@ -2069,7 +2070,7 @@
         <v>350</v>
       </c>
       <c r="E18" s="8">
-        <v>340</v>
+        <v>3</v>
       </c>
       <c r="F18" s="9">
         <v>0</v>
@@ -2085,44 +2086,44 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>9</v>
+      <c r="E20" t="s">
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="A21" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>